<commit_message>
20251216 Last check done before Review
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202512/Review 202512/Dataiku/C6RIP_EMS_2025-12-11_2025-12-11-23-06-11.xlsx
+++ b/GUI + Reviews/202512/Review 202512/Dataiku/C6RIP_EMS_2025-12-11_2025-12-11-23-06-11.xlsx
@@ -1,39 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202512/Review 202512/Dataiku/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_104BAF4BBDD2E81F8D9DC76BD18B417581B0FD9C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CAE5DA56-4DA9-4644-8168-70A3BAE8D05B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="selection" sheetId="1" r:id="rId1"/>
     <sheet name="inclusion" sheetId="2" r:id="rId2"/>
     <sheet name="exclusion" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">selection!$A$1:$H$61</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -439,8 +417,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,21 +481,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -555,7 +525,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -589,7 +559,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -624,10 +593,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -800,16 +768,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,7 +801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -861,7 +827,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -887,7 +853,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -913,7 +879,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -939,7 +905,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -965,7 +931,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -991,7 +957,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1017,7 +983,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1043,7 +1009,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1069,7 +1035,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1095,7 +1061,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1121,7 +1087,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1147,7 +1113,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1173,7 +1139,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1199,7 +1165,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1225,7 +1191,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1217,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1277,7 +1243,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1303,7 +1269,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1329,7 +1295,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1321,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1381,7 +1347,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1407,7 +1373,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1433,7 +1399,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1459,7 +1425,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1485,7 +1451,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1511,7 +1477,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1537,7 +1503,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1563,7 +1529,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1589,7 +1555,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1615,7 +1581,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1641,7 +1607,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1667,7 +1633,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1693,7 +1659,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1719,7 +1685,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1745,7 +1711,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1771,7 +1737,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1797,7 +1763,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1823,7 +1789,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1849,7 +1815,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1875,7 +1841,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1901,7 +1867,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1927,7 +1893,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -1953,7 +1919,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -1979,7 +1945,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2005,7 +1971,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2031,7 +1997,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2057,7 +2023,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2083,7 +2049,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>56</v>
       </c>
@@ -2109,7 +2075,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>57</v>
       </c>
@@ -2135,7 +2101,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>58</v>
       </c>
@@ -2161,7 +2127,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>59</v>
       </c>
@@ -2187,7 +2153,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>60</v>
       </c>
@@ -2213,7 +2179,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -2239,7 +2205,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>62</v>
       </c>
@@ -2265,7 +2231,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>63</v>
       </c>
@@ -2291,7 +2257,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>64</v>
       </c>
@@ -2317,7 +2283,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>65</v>
       </c>
@@ -2343,7 +2309,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>66</v>
       </c>
@@ -2369,7 +2335,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -2396,27 +2362,19 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H61" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H61">
-      <sortCondition ref="A1:A61"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFFEF00 PRIVATE</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2429,21 +2387,18 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFFEF00 PRIVATE</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2456,8 +2411,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFFEF00 PRIVATE</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>